<commit_message>
feat: Ordner Struktur figures angepasst
</commit_message>
<xml_diff>
--- a/Excel/Übersicht.xlsx
+++ b/Excel/Übersicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{76097CDE-4B74-4049-B171-ECFF49732868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{427CB0B1-5A7B-4A11-BE53-8AF56AE3199A}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{76097CDE-4B74-4049-B171-ECFF49732868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E30D1B-8F6E-4628-A14E-5074A1F22138}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="12" xr2:uid="{7A4F4436-C796-4ADD-B90F-7338F9426F96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="10" xr2:uid="{7A4F4436-C796-4ADD-B90F-7338F9426F96}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="2" state="hidden" r:id="rId1"/>
@@ -23,14 +23,15 @@
     <sheet name="RQ1" sheetId="5" r:id="rId8"/>
     <sheet name="RQ2" sheetId="6" state="hidden" r:id="rId9"/>
     <sheet name="RQ2 (2)" sheetId="14" r:id="rId10"/>
-    <sheet name="RQ3" sheetId="7" r:id="rId11"/>
-    <sheet name="Allgemeine Infos" sheetId="12" r:id="rId12"/>
-    <sheet name="Mapping RQ1 und RQ2" sheetId="17" r:id="rId13"/>
-    <sheet name="Quantitative Analyse" sheetId="13" state="hidden" r:id="rId14"/>
+    <sheet name="Zeitplan" sheetId="18" r:id="rId11"/>
+    <sheet name="RQ3" sheetId="7" r:id="rId12"/>
+    <sheet name="Allgemeine Infos" sheetId="12" r:id="rId13"/>
+    <sheet name="Mapping RQ1 und RQ2" sheetId="17" r:id="rId14"/>
+    <sheet name="Quantitative Analyse" sheetId="13" state="hidden" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Extraktion!$A$1:$V$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="12">'Mapping RQ1 und RQ2'!$A$1:$W$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="13">'Mapping RQ1 und RQ2'!$A$1:$W$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'RQ1'!$A$1:$W$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'RQ2 (2)'!$A$1:$W$12</definedName>
   </definedNames>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="1123">
   <si>
     <t>ID</t>
   </si>
@@ -7146,6 +7147,174 @@
   </si>
   <si>
     <t>RLHF/DPO erwähnt, aber kein RL-Anwendungsfall</t>
+  </si>
+  <si>
+    <t>Woche </t>
+  </si>
+  <si>
+    <t>Zeitraum </t>
+  </si>
+  <si>
+    <t>ToDo </t>
+  </si>
+  <si>
+    <t>Info </t>
+  </si>
+  <si>
+    <t>Woche 1 </t>
+  </si>
+  <si>
+    <t>03. Nov </t>
+  </si>
+  <si>
+    <t>Suchstrings finalisieren, Basispaper prüfen </t>
+  </si>
+  <si>
+    <t>Mapping Study Start gemäß Petersen/Wohlin </t>
+  </si>
+  <si>
+    <t>Woche 2 </t>
+  </si>
+  <si>
+    <t>10. Nov </t>
+  </si>
+  <si>
+    <t>Paper-Sichtung &amp; erste Datenextraktion </t>
+  </si>
+  <si>
+    <t>Datenextraktion nach Tabelle 3.2 </t>
+  </si>
+  <si>
+    <t>Woche 3 </t>
+  </si>
+  <si>
+    <t>17. Nov </t>
+  </si>
+  <si>
+    <t>Paper-Analyse fortsetzen, Extraktion vervollständigen </t>
+  </si>
+  <si>
+    <t>Analyse der KI-Ansätze </t>
+  </si>
+  <si>
+    <t>Woche 4 </t>
+  </si>
+  <si>
+    <t>24. Nov </t>
+  </si>
+  <si>
+    <t>Datenextraktion abschließen, Kategorien bilden </t>
+  </si>
+  <si>
+    <t>Kategorien gemäß Platform-Engineering-Bereichen </t>
+  </si>
+  <si>
+    <t>Woche 5 </t>
+  </si>
+  <si>
+    <t>01. Dez </t>
+  </si>
+  <si>
+    <t>Datensynthese vorbereiten </t>
+  </si>
+  <si>
+    <t>Synthesis entlang RQs </t>
+  </si>
+  <si>
+    <t>Woche 6 </t>
+  </si>
+  <si>
+    <t>08. Dez </t>
+  </si>
+  <si>
+    <t>Quantitative Analyse erstellen </t>
+  </si>
+  <si>
+    <t>Statistische Übersicht erstellen </t>
+  </si>
+  <si>
+    <t>Woche 7 </t>
+  </si>
+  <si>
+    <t>15. Dez </t>
+  </si>
+  <si>
+    <t>Mapping Study Kapitel schreiben </t>
+  </si>
+  <si>
+    <t>Kapitel 4 ausformulieren </t>
+  </si>
+  <si>
+    <t>Woche 8 </t>
+  </si>
+  <si>
+    <t>22. Dez </t>
+  </si>
+  <si>
+    <t>Mapping Study finalisieren </t>
+  </si>
+  <si>
+    <t>Review + Konsistenzcheck </t>
+  </si>
+  <si>
+    <t>Woche 9 </t>
+  </si>
+  <si>
+    <t>29. Dez </t>
+  </si>
+  <si>
+    <t>Start Framework-Konzeption (Kriterien sammeln) </t>
+  </si>
+  <si>
+    <t>RQ3 Beginn </t>
+  </si>
+  <si>
+    <t>Woche 10 </t>
+  </si>
+  <si>
+    <t>05. Jan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Framework strukturieren </t>
+  </si>
+  <si>
+    <t>Kriterien definieren</t>
+  </si>
+  <si>
+    <t>Woche 11 </t>
+  </si>
+  <si>
+    <t>12. Jan </t>
+  </si>
+  <si>
+    <t>Framework ausarbeiten </t>
+  </si>
+  <si>
+    <t>Kapitel 5 schreiben </t>
+  </si>
+  <si>
+    <t>Woche 12 </t>
+  </si>
+  <si>
+    <t>19. Jan </t>
+  </si>
+  <si>
+    <t>Diskussion + Beantwortung RQs schreiben </t>
+  </si>
+  <si>
+    <t>Kapitel 6 </t>
+  </si>
+  <si>
+    <t>Woche 13 </t>
+  </si>
+  <si>
+    <t>26. Jan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feinschliff, Zusammenfassung  und Ausblick </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA finalisieren </t>
   </si>
 </sst>
 </file>
@@ -7281,7 +7450,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7327,6 +7496,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7973,7 +8148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8321,6 +8496,19 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -8354,28 +8542,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8396,19 +8575,16 @@
     <xf numFmtId="49" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -9249,11 +9425,11 @@
       <c r="D5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="121" t="s">
+      <c r="G5" s="126" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
     </row>
     <row r="6" spans="1:9" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21" t="s">
@@ -9283,11 +9459,11 @@
         <f>"Rückwärts aus " &amp; A2</f>
         <v>Rückwärts aus P1</v>
       </c>
-      <c r="G7" s="122" t="s">
+      <c r="G7" s="127" t="s">
         <v>284</v>
       </c>
-      <c r="H7" s="122"/>
-      <c r="I7" s="122"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
     </row>
     <row r="8" spans="1:9" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -9303,9 +9479,9 @@
         <f>"Rückwärts aus " &amp; A2</f>
         <v>Rückwärts aus P1</v>
       </c>
-      <c r="G8" s="122"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
     </row>
     <row r="9" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
@@ -9615,7 +9791,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A6" sqref="A6:W8"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9717,7 +9893,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="25" x14ac:dyDescent="0.35">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="133" t="s">
         <v>255</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -9768,7 +9944,7 @@
       <c r="W2" s="27"/>
     </row>
     <row r="3" spans="1:23" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="129"/>
+      <c r="A3" s="134"/>
       <c r="B3" s="33" t="s">
         <v>323</v>
       </c>
@@ -9825,7 +10001,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="129"/>
+      <c r="A4" s="134"/>
       <c r="B4" s="33" t="s">
         <v>257</v>
       </c>
@@ -9878,7 +10054,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="129"/>
+      <c r="A5" s="134"/>
       <c r="B5" s="35" t="s">
         <v>326</v>
       </c>
@@ -9917,7 +10093,7 @@
       <c r="W5" s="30"/>
     </row>
     <row r="6" spans="1:23" ht="50" x14ac:dyDescent="0.35">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="133" t="s">
         <v>687</v>
       </c>
       <c r="B6" s="31" t="s">
@@ -9949,7 +10125,7 @@
         <v>716</v>
       </c>
       <c r="L6" s="26"/>
-      <c r="M6" s="149" t="s">
+      <c r="M6" s="124" t="s">
         <v>1005</v>
       </c>
       <c r="N6" s="26" t="s">
@@ -9973,7 +10149,7 @@
       <c r="T6" s="26" t="s">
         <v>710</v>
       </c>
-      <c r="U6" s="149" t="s">
+      <c r="U6" s="124" t="s">
         <v>1046</v>
       </c>
       <c r="V6" s="79" t="s">
@@ -9984,7 +10160,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="50" x14ac:dyDescent="0.35">
-      <c r="A7" s="129"/>
+      <c r="A7" s="134"/>
       <c r="B7" s="33" t="s">
         <v>642</v>
       </c>
@@ -10033,18 +10209,18 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="131"/>
+      <c r="A8" s="136"/>
       <c r="B8" s="35" t="s">
         <v>592</v>
       </c>
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="122" t="s">
         <v>1065</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="F8" s="148" t="s">
+      <c r="F8" s="123" t="s">
         <v>1066</v>
       </c>
       <c r="G8" s="29"/>
@@ -10061,14 +10237,14 @@
       <c r="N8" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="O8" s="148" t="s">
+      <c r="O8" s="123" t="s">
         <v>396</v>
       </c>
       <c r="P8" s="29" t="s">
         <v>444</v>
       </c>
       <c r="Q8" s="29"/>
-      <c r="R8" s="148" t="s">
+      <c r="R8" s="123" t="s">
         <v>718</v>
       </c>
       <c r="S8" s="29" t="s">
@@ -10082,7 +10258,7 @@
       <c r="W8" s="30"/>
     </row>
     <row r="9" spans="1:23" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="134" t="s">
         <v>688</v>
       </c>
       <c r="B9" s="31" t="s">
@@ -10091,7 +10267,7 @@
       <c r="C9" s="32" t="s">
         <v>965</v>
       </c>
-      <c r="D9" s="150" t="s">
+      <c r="D9" s="125" t="s">
         <v>721</v>
       </c>
       <c r="E9" s="26" t="s">
@@ -10147,7 +10323,7 @@
       <c r="W9" s="27"/>
     </row>
     <row r="10" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="129"/>
+      <c r="A10" s="134"/>
       <c r="B10" s="113" t="s">
         <v>962</v>
       </c>
@@ -10188,7 +10364,7 @@
       <c r="W10" s="117"/>
     </row>
     <row r="11" spans="1:23" ht="50" x14ac:dyDescent="0.35">
-      <c r="A11" s="129"/>
+      <c r="A11" s="134"/>
       <c r="B11" s="33" t="s">
         <v>963</v>
       </c>
@@ -10239,7 +10415,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="131"/>
+      <c r="A12" s="136"/>
       <c r="B12" s="35" t="s">
         <v>964</v>
       </c>
@@ -10288,7 +10464,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A16" s="146" t="s">
+      <c r="A16" s="121" t="s">
         <v>1065</v>
       </c>
     </row>
@@ -10313,6 +10489,221 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7013A05C-DE60-48CF-8EAC-BA1D4A04F40F}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="4" width="50.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="69" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="151" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B2" s="151" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C2" s="151" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D2" s="151" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="151" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B3" s="151" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C3" s="151" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D3" s="151" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="151" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B4" s="151" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C4" s="151" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D4" s="151" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="151" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B5" s="151" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C5" s="151" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D5" s="151" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="151" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B6" s="151" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C6" s="151" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D6" s="151" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="74" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="74" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="74" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="74" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D10" s="74" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="74" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C11" s="74" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="74" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D12" s="74" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="74" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="74" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C14" s="74" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C706DF66-24ED-41CC-A436-656F740ECEA8}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -10382,7 +10773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4371E66-F69A-4A6E-8DB3-95C6DD4CBD0F}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -10413,31 +10804,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="139" t="s">
         <v>495</v>
       </c>
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="142" t="s">
         <v>496</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="133" t="s">
+      <c r="C2" s="145"/>
+      <c r="D2" s="149" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="136"/>
-      <c r="B3" s="141"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="132"/>
+      <c r="A3" s="141"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="148"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="137"/>
-      <c r="B4" s="142"/>
-      <c r="C4" s="145"/>
-      <c r="D4" s="134"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="150"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="135" t="s">
+      <c r="A5" s="139" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="58" t="s">
@@ -10451,7 +10842,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="136"/>
+      <c r="A6" s="141"/>
       <c r="B6" s="53" t="s">
         <v>499</v>
       </c>
@@ -10463,7 +10854,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="136"/>
+      <c r="A7" s="141"/>
       <c r="B7" s="53" t="s">
         <v>501</v>
       </c>
@@ -10475,13 +10866,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="137"/>
+      <c r="A8" s="140"/>
       <c r="B8" s="62"/>
       <c r="C8" s="63"/>
       <c r="D8" s="64"/>
     </row>
     <row r="9" spans="1:4" ht="25" x14ac:dyDescent="0.35">
-      <c r="A9" s="135" t="s">
+      <c r="A9" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="58" t="s">
@@ -10495,7 +10886,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="137"/>
+      <c r="A10" s="140"/>
       <c r="B10" s="82" t="s">
         <v>506</v>
       </c>
@@ -10507,7 +10898,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="137" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="88" t="s">
@@ -10521,13 +10912,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="139"/>
+      <c r="A12" s="138"/>
       <c r="B12" s="89"/>
       <c r="C12" s="63"/>
       <c r="D12" s="64"/>
     </row>
     <row r="13" spans="1:4" ht="25" x14ac:dyDescent="0.35">
-      <c r="A13" s="135" t="s">
+      <c r="A13" s="139" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="85" t="s">
@@ -10541,7 +10932,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="136"/>
+      <c r="A14" s="141"/>
       <c r="B14" s="53" t="s">
         <v>514</v>
       </c>
@@ -10553,7 +10944,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="136"/>
+      <c r="A15" s="141"/>
       <c r="B15" s="53" t="s">
         <v>474</v>
       </c>
@@ -10565,25 +10956,25 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="25" x14ac:dyDescent="0.35">
-      <c r="A16" s="136"/>
-      <c r="B16" s="141"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="52" t="s">
         <v>519</v>
       </c>
-      <c r="D16" s="132" t="s">
+      <c r="D16" s="148" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="136"/>
-      <c r="B17" s="141"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="52" t="s">
         <v>520</v>
       </c>
-      <c r="D17" s="132"/>
+      <c r="D17" s="148"/>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="137"/>
+      <c r="A18" s="140"/>
       <c r="B18" s="62"/>
       <c r="C18" s="63" t="s">
         <v>522</v>
@@ -10593,7 +10984,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="138" t="s">
+      <c r="A19" s="137" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="88" t="s">
@@ -10607,13 +10998,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="139"/>
+      <c r="A20" s="138"/>
       <c r="B20" s="89"/>
       <c r="C20" s="63"/>
       <c r="D20" s="64"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="139" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="58" t="s">
@@ -10627,37 +11018,37 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="137"/>
+      <c r="A22" s="140"/>
       <c r="B22" s="62"/>
       <c r="C22" s="63"/>
       <c r="D22" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFE91FF-44F0-441B-9BF4-83ADF34482BD}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10770,7 +11161,7 @@
       <c r="AH1" s="93"/>
     </row>
     <row r="2" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="133" t="s">
         <v>321</v>
       </c>
       <c r="B2" s="95" t="s">
@@ -10832,7 +11223,7 @@
       <c r="AH2" s="6"/>
     </row>
     <row r="3" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="129"/>
+      <c r="A3" s="134"/>
       <c r="B3" s="96" t="s">
         <v>252</v>
       </c>
@@ -10906,7 +11297,7 @@
       <c r="AH3" s="6"/>
     </row>
     <row r="4" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A4" s="129"/>
+      <c r="A4" s="134"/>
       <c r="B4" s="96" t="s">
         <v>264</v>
       </c>
@@ -10974,7 +11365,7 @@
       <c r="AH4" s="6"/>
     </row>
     <row r="5" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="129"/>
+      <c r="A5" s="134"/>
       <c r="B5" s="96" t="s">
         <v>1016</v>
       </c>
@@ -11048,7 +11439,7 @@
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:34" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="129"/>
+      <c r="A6" s="134"/>
       <c r="B6" s="97" t="s">
         <v>1017</v>
       </c>
@@ -11116,7 +11507,7 @@
       <c r="AH6" s="6"/>
     </row>
     <row r="7" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="130" t="s">
         <v>320</v>
       </c>
       <c r="B7" s="95" t="s">
@@ -11194,7 +11585,7 @@
       <c r="AH7" s="6"/>
     </row>
     <row r="8" spans="1:34" ht="75" x14ac:dyDescent="0.35">
-      <c r="A8" s="126"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="96" t="s">
         <v>998</v>
       </c>
@@ -11268,7 +11659,7 @@
       <c r="AH8" s="6"/>
     </row>
     <row r="9" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="126"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="96" t="s">
         <v>1018</v>
       </c>
@@ -11338,7 +11729,7 @@
       <c r="AH9" s="6"/>
     </row>
     <row r="10" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A10" s="126"/>
+      <c r="A10" s="131"/>
       <c r="B10" s="96" t="s">
         <v>1019</v>
       </c>
@@ -11408,7 +11799,7 @@
       <c r="AH10" s="6"/>
     </row>
     <row r="11" spans="1:34" ht="63" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="127"/>
+      <c r="A11" s="132"/>
       <c r="B11" s="98" t="s">
         <v>1020</v>
       </c>
@@ -11465,7 +11856,7 @@
       </c>
     </row>
     <row r="12" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="133" t="s">
         <v>687</v>
       </c>
       <c r="B12" s="31" t="s">
@@ -11497,7 +11888,7 @@
         <v>716</v>
       </c>
       <c r="L12" s="26"/>
-      <c r="M12" s="149" t="s">
+      <c r="M12" s="124" t="s">
         <v>1005</v>
       </c>
       <c r="N12" s="26" t="s">
@@ -11521,7 +11912,7 @@
       <c r="T12" s="26" t="s">
         <v>710</v>
       </c>
-      <c r="U12" s="149" t="s">
+      <c r="U12" s="124" t="s">
         <v>1046</v>
       </c>
       <c r="V12" s="79" t="s">
@@ -11532,7 +11923,7 @@
       </c>
     </row>
     <row r="13" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A13" s="129"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="33" t="s">
         <v>642</v>
       </c>
@@ -11581,18 +11972,18 @@
       </c>
     </row>
     <row r="14" spans="1:34" ht="38" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="131"/>
+      <c r="A14" s="136"/>
       <c r="B14" s="35" t="s">
         <v>592</v>
       </c>
-      <c r="C14" s="147" t="s">
+      <c r="C14" s="122" t="s">
         <v>1065</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="F14" s="148" t="s">
+      <c r="F14" s="123" t="s">
         <v>1066</v>
       </c>
       <c r="G14" s="29"/>
@@ -11609,14 +12000,14 @@
       <c r="N14" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="O14" s="148" t="s">
+      <c r="O14" s="123" t="s">
         <v>396</v>
       </c>
       <c r="P14" s="29" t="s">
         <v>444</v>
       </c>
       <c r="Q14" s="29"/>
-      <c r="R14" s="148" t="s">
+      <c r="R14" s="123" t="s">
         <v>718</v>
       </c>
       <c r="S14" s="29" t="s">
@@ -11803,7 +12194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DE2F3E-D1CE-4B93-B6DF-12C89A233AC2}">
   <dimension ref="A1:R16"/>
   <sheetViews>
@@ -13435,13 +13826,13 @@
       <c r="D1" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
     </row>
     <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
@@ -14689,18 +15080,18 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B13" s="124"/>
-      <c r="C13" s="124"/>
+      <c r="B13" s="129"/>
+      <c r="C13" s="129"/>
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B14" s="124"/>
-      <c r="C14" s="124"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:22" ht="100.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="124"/>
-      <c r="C15" s="124"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="129"/>
       <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
@@ -14844,7 +15235,7 @@
       <c r="AH1" s="93"/>
     </row>
     <row r="2" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="133" t="s">
         <v>321</v>
       </c>
       <c r="B2" s="95" t="s">
@@ -14906,7 +15297,7 @@
       <c r="AH2" s="6"/>
     </row>
     <row r="3" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="129"/>
+      <c r="A3" s="134"/>
       <c r="B3" s="96" t="s">
         <v>252</v>
       </c>
@@ -14980,7 +15371,7 @@
       <c r="AH3" s="6"/>
     </row>
     <row r="4" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A4" s="129"/>
+      <c r="A4" s="134"/>
       <c r="B4" s="96" t="s">
         <v>264</v>
       </c>
@@ -15048,7 +15439,7 @@
       <c r="AH4" s="6"/>
     </row>
     <row r="5" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="129"/>
+      <c r="A5" s="134"/>
       <c r="B5" s="96" t="s">
         <v>1016</v>
       </c>
@@ -15122,7 +15513,7 @@
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:34" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="129"/>
+      <c r="A6" s="134"/>
       <c r="B6" s="97" t="s">
         <v>1017</v>
       </c>
@@ -15190,7 +15581,7 @@
       <c r="AH6" s="6"/>
     </row>
     <row r="7" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="130" t="s">
         <v>320</v>
       </c>
       <c r="B7" s="95" t="s">
@@ -15268,7 +15659,7 @@
       <c r="AH7" s="6"/>
     </row>
     <row r="8" spans="1:34" ht="75" x14ac:dyDescent="0.35">
-      <c r="A8" s="126"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="96" t="s">
         <v>998</v>
       </c>
@@ -15342,7 +15733,7 @@
       <c r="AH8" s="6"/>
     </row>
     <row r="9" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="126"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="96" t="s">
         <v>1018</v>
       </c>
@@ -15412,7 +15803,7 @@
       <c r="AH9" s="6"/>
     </row>
     <row r="10" spans="1:34" ht="50" x14ac:dyDescent="0.35">
-      <c r="A10" s="126"/>
+      <c r="A10" s="131"/>
       <c r="B10" s="96" t="s">
         <v>1019</v>
       </c>
@@ -15482,7 +15873,7 @@
       <c r="AH10" s="6"/>
     </row>
     <row r="11" spans="1:34" ht="63" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="127"/>
+      <c r="A11" s="132"/>
       <c r="B11" s="98" t="s">
         <v>1020</v>
       </c>
@@ -15822,7 +16213,7 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="25" x14ac:dyDescent="0.35">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="133" t="s">
         <v>255</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -15896,7 +16287,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="129"/>
+      <c r="A3" s="134"/>
       <c r="B3" s="33" t="s">
         <v>323</v>
       </c>
@@ -15968,7 +16359,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="129"/>
+      <c r="A4" s="134"/>
       <c r="B4" s="33" t="s">
         <v>257</v>
       </c>
@@ -16040,7 +16431,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="130"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="35" t="s">
         <v>326</v>
       </c>

</xml_diff>

<commit_message>
feat: Grundlagen & 04_02
</commit_message>
<xml_diff>
--- a/Excel/Übersicht.xlsx
+++ b/Excel/Übersicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BADDE5A-316A-CA40-867C-F5A5795F0F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33403420-5907-DA46-B7C0-E41E2D3232BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="14" xr2:uid="{7A4F4436-C796-4ADD-B90F-7338F9426F96}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10" xr2:uid="{7A4F4436-C796-4ADD-B90F-7338F9426F96}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="2" state="hidden" r:id="rId1"/>
@@ -8540,6 +8540,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -8573,28 +8577,19 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8615,10 +8610,15 @@
     <xf numFmtId="49" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -9459,11 +9459,11 @@
       <c r="D5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="126" t="s">
+      <c r="G5" s="128" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
     </row>
     <row r="6" spans="1:9" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -9493,11 +9493,11 @@
         <f>"Rückwärts aus " &amp; A2</f>
         <v>Rückwärts aus P1</v>
       </c>
-      <c r="G7" s="127" t="s">
+      <c r="G7" s="129" t="s">
         <v>284</v>
       </c>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
     </row>
     <row r="8" spans="1:9" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -9513,9 +9513,9 @@
         <f>"Rückwärts aus " &amp; A2</f>
         <v>Rückwärts aus P1</v>
       </c>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
     </row>
     <row r="9" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -9927,7 +9927,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="28" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>255</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -9978,7 +9978,7 @@
       <c r="W2" s="27"/>
     </row>
     <row r="3" spans="1:23" ht="98" x14ac:dyDescent="0.2">
-      <c r="A3" s="134"/>
+      <c r="A3" s="136"/>
       <c r="B3" s="33" t="s">
         <v>323</v>
       </c>
@@ -10035,7 +10035,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="70" x14ac:dyDescent="0.2">
-      <c r="A4" s="134"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="33" t="s">
         <v>257</v>
       </c>
@@ -10081,12 +10081,12 @@
       </c>
       <c r="U4" s="25"/>
       <c r="V4" s="25"/>
-      <c r="W4" s="151" t="s">
+      <c r="W4" s="126" t="s">
         <v>1129</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="134"/>
+      <c r="A5" s="136"/>
       <c r="B5" s="35" t="s">
         <v>326</v>
       </c>
@@ -10125,7 +10125,7 @@
       <c r="W5" s="30"/>
     </row>
     <row r="6" spans="1:23" ht="56" x14ac:dyDescent="0.2">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="135" t="s">
         <v>687</v>
       </c>
       <c r="B6" s="31" t="s">
@@ -10192,7 +10192,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="56" x14ac:dyDescent="0.2">
-      <c r="A7" s="134"/>
+      <c r="A7" s="136"/>
       <c r="B7" s="33" t="s">
         <v>642</v>
       </c>
@@ -10241,7 +10241,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
+      <c r="A8" s="138"/>
       <c r="B8" s="35" t="s">
         <v>592</v>
       </c>
@@ -10290,7 +10290,7 @@
       <c r="W8" s="30"/>
     </row>
     <row r="9" spans="1:23" ht="42" x14ac:dyDescent="0.2">
-      <c r="A9" s="134" t="s">
+      <c r="A9" s="136" t="s">
         <v>688</v>
       </c>
       <c r="B9" s="31" t="s">
@@ -10355,7 +10355,7 @@
       <c r="W9" s="27"/>
     </row>
     <row r="10" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="134"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="113" t="s">
         <v>962</v>
       </c>
@@ -10396,7 +10396,7 @@
       <c r="W10" s="117"/>
     </row>
     <row r="11" spans="1:23" ht="42" x14ac:dyDescent="0.2">
-      <c r="A11" s="134"/>
+      <c r="A11" s="136"/>
       <c r="B11" s="33" t="s">
         <v>963</v>
       </c>
@@ -10445,7 +10445,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
+      <c r="A12" s="138"/>
       <c r="B12" s="35" t="s">
         <v>964</v>
       </c>
@@ -10520,8 +10520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7013A05C-DE60-48CF-8EAC-BA1D4A04F40F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10615,16 +10615,16 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="125" t="s">
         <v>1090</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="125" t="s">
         <v>1091</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="125" t="s">
         <v>1092</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="125" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -10832,31 +10832,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="141" t="s">
         <v>495</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="144" t="s">
         <v>496</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="138" t="s">
+      <c r="C2" s="147"/>
+      <c r="D2" s="151" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="141"/>
-      <c r="B3" s="146"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="137"/>
+      <c r="A3" s="143"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="150"/>
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="142"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="139"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="152"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="140" t="s">
+      <c r="A5" s="141" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="58" t="s">
@@ -10870,7 +10870,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="141"/>
+      <c r="A6" s="143"/>
       <c r="B6" s="53" t="s">
         <v>499</v>
       </c>
@@ -10882,7 +10882,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="141"/>
+      <c r="A7" s="143"/>
       <c r="B7" s="53" t="s">
         <v>501</v>
       </c>
@@ -10900,7 +10900,7 @@
       <c r="D8" s="64"/>
     </row>
     <row r="9" spans="1:4" ht="28" x14ac:dyDescent="0.2">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="141" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="58" t="s">
@@ -10926,7 +10926,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="143" t="s">
+      <c r="A11" s="139" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="88" t="s">
@@ -10940,13 +10940,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
+      <c r="A12" s="140"/>
       <c r="B12" s="89"/>
       <c r="C12" s="63"/>
       <c r="D12" s="64"/>
     </row>
     <row r="13" spans="1:4" ht="28" x14ac:dyDescent="0.2">
-      <c r="A13" s="140" t="s">
+      <c r="A13" s="141" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="85" t="s">
@@ -10960,7 +10960,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="141"/>
+      <c r="A14" s="143"/>
       <c r="B14" s="53" t="s">
         <v>514</v>
       </c>
@@ -10972,7 +10972,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="141"/>
+      <c r="A15" s="143"/>
       <c r="B15" s="53" t="s">
         <v>474</v>
       </c>
@@ -10984,22 +10984,22 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="141"/>
-      <c r="B16" s="146"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="145"/>
       <c r="C16" s="52" t="s">
         <v>519</v>
       </c>
-      <c r="D16" s="137" t="s">
+      <c r="D16" s="150" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="141"/>
-      <c r="B17" s="146"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="145"/>
       <c r="C17" s="52" t="s">
         <v>520</v>
       </c>
-      <c r="D17" s="137"/>
+      <c r="D17" s="150"/>
     </row>
     <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="142"/>
@@ -11012,7 +11012,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="139" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="88" t="s">
@@ -11026,13 +11026,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="144"/>
+      <c r="A20" s="140"/>
       <c r="B20" s="89"/>
       <c r="C20" s="63"/>
       <c r="D20" s="64"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="140" t="s">
+      <c r="A21" s="141" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="58" t="s">
@@ -11053,18 +11053,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11074,9 +11074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFE91FF-44F0-441B-9BF4-83ADF34482BD}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="A7:XFD15"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11189,7 +11189,7 @@
       <c r="AH1" s="93"/>
     </row>
     <row r="2" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>321</v>
       </c>
       <c r="B2" s="95" t="s">
@@ -11251,7 +11251,7 @@
       <c r="AH2" s="6"/>
     </row>
     <row r="3" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A3" s="134"/>
+      <c r="A3" s="136"/>
       <c r="B3" s="96" t="s">
         <v>252</v>
       </c>
@@ -11325,7 +11325,7 @@
       <c r="AH3" s="6"/>
     </row>
     <row r="4" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A4" s="134"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="96" t="s">
         <v>264</v>
       </c>
@@ -11392,8 +11392,8 @@
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
     </row>
-    <row r="5" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A5" s="134"/>
+    <row r="5" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+      <c r="A5" s="136"/>
       <c r="B5" s="96" t="s">
         <v>1015</v>
       </c>
@@ -11467,7 +11467,7 @@
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:34" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="136"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="97" t="s">
         <v>1016</v>
       </c>
@@ -11535,7 +11535,7 @@
       <c r="AH6" s="6"/>
     </row>
     <row r="7" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="135" t="s">
         <v>320</v>
       </c>
       <c r="B7" s="95" t="s">
@@ -11613,7 +11613,7 @@
       <c r="AH7" s="6"/>
     </row>
     <row r="8" spans="1:34" ht="84" x14ac:dyDescent="0.2">
-      <c r="A8" s="134"/>
+      <c r="A8" s="136"/>
       <c r="B8" s="96" t="s">
         <v>997</v>
       </c>
@@ -11687,7 +11687,7 @@
       <c r="AH8" s="6"/>
     </row>
     <row r="9" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A9" s="134"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="96" t="s">
         <v>1017</v>
       </c>
@@ -11757,7 +11757,7 @@
       <c r="AH9" s="6"/>
     </row>
     <row r="10" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A10" s="134"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="96" t="s">
         <v>1018</v>
       </c>
@@ -11827,7 +11827,7 @@
       <c r="AH10" s="6"/>
     </row>
     <row r="11" spans="1:34" ht="71" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="136"/>
+      <c r="A11" s="138"/>
       <c r="B11" s="98" t="s">
         <v>1019</v>
       </c>
@@ -11884,7 +11884,7 @@
       </c>
     </row>
     <row r="12" spans="1:34" ht="28" x14ac:dyDescent="0.2">
-      <c r="A12" s="133" t="s">
+      <c r="A12" s="135" t="s">
         <v>255</v>
       </c>
       <c r="B12" s="31" t="s">
@@ -11933,7 +11933,7 @@
       <c r="W12" s="27"/>
     </row>
     <row r="13" spans="1:34" ht="42" x14ac:dyDescent="0.2">
-      <c r="A13" s="134"/>
+      <c r="A13" s="136"/>
       <c r="B13" s="33" t="s">
         <v>323</v>
       </c>
@@ -11990,7 +11990,7 @@
       </c>
     </row>
     <row r="14" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A14" s="134"/>
+      <c r="A14" s="136"/>
       <c r="B14" s="33" t="s">
         <v>257</v>
       </c>
@@ -12043,7 +12043,7 @@
       </c>
     </row>
     <row r="15" spans="1:34" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="136"/>
+      <c r="A15" s="138"/>
       <c r="B15" s="35" t="s">
         <v>326</v>
       </c>
@@ -12082,7 +12082,7 @@
       <c r="W15" s="30"/>
     </row>
     <row r="16" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A16" s="133" t="s">
+      <c r="A16" s="135" t="s">
         <v>687</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -12149,7 +12149,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" ht="56" x14ac:dyDescent="0.2">
-      <c r="A17" s="134"/>
+      <c r="A17" s="136"/>
       <c r="B17" s="33" t="s">
         <v>642</v>
       </c>
@@ -12198,7 +12198,7 @@
       </c>
     </row>
     <row r="18" spans="1:33" ht="43" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="136"/>
+      <c r="A18" s="138"/>
       <c r="B18" s="35" t="s">
         <v>592</v>
       </c>
@@ -12247,7 +12247,7 @@
       <c r="W18" s="30"/>
     </row>
     <row r="19" spans="1:33" ht="42" x14ac:dyDescent="0.2">
-      <c r="A19" s="133" t="s">
+      <c r="A19" s="135" t="s">
         <v>688</v>
       </c>
       <c r="B19" s="31" t="s">
@@ -12312,7 +12312,7 @@
       <c r="W19" s="27"/>
     </row>
     <row r="20" spans="1:33" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="134"/>
+      <c r="A20" s="136"/>
       <c r="B20" s="113" t="s">
         <v>962</v>
       </c>
@@ -12352,8 +12352,8 @@
       </c>
       <c r="W20" s="117"/>
     </row>
-    <row r="21" spans="1:33" ht="56" x14ac:dyDescent="0.2">
-      <c r="A21" s="134"/>
+    <row r="21" spans="1:33" ht="42" x14ac:dyDescent="0.2">
+      <c r="A21" s="136"/>
       <c r="B21" s="33" t="s">
         <v>963</v>
       </c>
@@ -12402,7 +12402,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="136"/>
+      <c r="A22" s="138"/>
       <c r="B22" s="35" t="s">
         <v>964</v>
       </c>
@@ -12649,8 +12649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE6C088-7B1A-724F-96D6-11C56C9BF066}">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -12660,72 +12660,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="152" t="s">
+      <c r="C1" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="152" t="s">
+      <c r="D1" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="152" t="s">
+      <c r="E1" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="152" t="s">
+      <c r="F1" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="152" t="s">
+      <c r="G1" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="152" t="s">
+      <c r="H1" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="152" t="s">
+      <c r="I1" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="152" t="s">
+      <c r="J1" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="152" t="s">
+      <c r="K1" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="152" t="s">
+      <c r="L1" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="152" t="s">
+      <c r="M1" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="152" t="s">
+      <c r="N1" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="152" t="s">
+      <c r="O1" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="152" t="s">
+      <c r="P1" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="152" t="s">
+      <c r="Q1" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="152" t="s">
+      <c r="R1" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="152" t="s">
+      <c r="S1" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="152" t="s">
+      <c r="T1" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="152" t="s">
+      <c r="U1" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="152" t="s">
+      <c r="V1" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="152" t="s">
+      <c r="W1" s="127" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="84" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>320</v>
       </c>
       <c r="B2" s="95" t="s">
@@ -12803,7 +12803,7 @@
       <c r="AH2" s="6"/>
     </row>
     <row r="3" spans="1:34" ht="126" x14ac:dyDescent="0.2">
-      <c r="A3" s="134"/>
+      <c r="A3" s="136"/>
       <c r="B3" s="96" t="s">
         <v>997</v>
       </c>
@@ -12877,7 +12877,7 @@
       <c r="AH3" s="6"/>
     </row>
     <row r="4" spans="1:34" ht="98" x14ac:dyDescent="0.2">
-      <c r="A4" s="134"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="96" t="s">
         <v>1017</v>
       </c>
@@ -12947,7 +12947,7 @@
       <c r="AH4" s="6"/>
     </row>
     <row r="5" spans="1:34" ht="84" x14ac:dyDescent="0.2">
-      <c r="A5" s="134"/>
+      <c r="A5" s="136"/>
       <c r="B5" s="96" t="s">
         <v>1018</v>
       </c>
@@ -13017,7 +13017,7 @@
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:34" ht="99" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="136"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="98" t="s">
         <v>1019</v>
       </c>
@@ -13074,7 +13074,7 @@
       </c>
     </row>
     <row r="7" spans="1:34" ht="28" x14ac:dyDescent="0.2">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="135" t="s">
         <v>255</v>
       </c>
       <c r="B7" s="31" t="s">
@@ -13125,7 +13125,7 @@
       <c r="W7" s="27"/>
     </row>
     <row r="8" spans="1:34" ht="98" x14ac:dyDescent="0.2">
-      <c r="A8" s="134"/>
+      <c r="A8" s="136"/>
       <c r="B8" s="33" t="s">
         <v>323</v>
       </c>
@@ -13182,7 +13182,7 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="98" x14ac:dyDescent="0.2">
-      <c r="A9" s="134"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="33" t="s">
         <v>257</v>
       </c>
@@ -13233,7 +13233,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" ht="43" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="136"/>
+      <c r="A10" s="138"/>
       <c r="B10" s="35" t="s">
         <v>326</v>
       </c>
@@ -14913,13 +14913,13 @@
       <c r="D1" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -16167,18 +16167,18 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B13" s="129"/>
-      <c r="C13" s="129"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="131"/>
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B14" s="129"/>
-      <c r="C14" s="129"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:22" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="129"/>
-      <c r="C15" s="129"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="131"/>
       <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -16322,7 +16322,7 @@
       <c r="AH1" s="93"/>
     </row>
     <row r="2" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>321</v>
       </c>
       <c r="B2" s="95" t="s">
@@ -16384,7 +16384,7 @@
       <c r="AH2" s="6"/>
     </row>
     <row r="3" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A3" s="134"/>
+      <c r="A3" s="136"/>
       <c r="B3" s="96" t="s">
         <v>252</v>
       </c>
@@ -16458,7 +16458,7 @@
       <c r="AH3" s="6"/>
     </row>
     <row r="4" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A4" s="134"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="96" t="s">
         <v>264</v>
       </c>
@@ -16526,7 +16526,7 @@
       <c r="AH4" s="6"/>
     </row>
     <row r="5" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A5" s="134"/>
+      <c r="A5" s="136"/>
       <c r="B5" s="96" t="s">
         <v>1015</v>
       </c>
@@ -16600,7 +16600,7 @@
       <c r="AH5" s="6"/>
     </row>
     <row r="6" spans="1:34" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="134"/>
+      <c r="A6" s="136"/>
       <c r="B6" s="97" t="s">
         <v>1016</v>
       </c>
@@ -16668,7 +16668,7 @@
       <c r="AH6" s="6"/>
     </row>
     <row r="7" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="132" t="s">
         <v>320</v>
       </c>
       <c r="B7" s="95" t="s">
@@ -16746,7 +16746,7 @@
       <c r="AH7" s="6"/>
     </row>
     <row r="8" spans="1:34" ht="84" x14ac:dyDescent="0.2">
-      <c r="A8" s="131"/>
+      <c r="A8" s="133"/>
       <c r="B8" s="96" t="s">
         <v>997</v>
       </c>
@@ -16820,7 +16820,7 @@
       <c r="AH8" s="6"/>
     </row>
     <row r="9" spans="1:34" ht="70" x14ac:dyDescent="0.2">
-      <c r="A9" s="131"/>
+      <c r="A9" s="133"/>
       <c r="B9" s="96" t="s">
         <v>1017</v>
       </c>
@@ -16890,7 +16890,7 @@
       <c r="AH9" s="6"/>
     </row>
     <row r="10" spans="1:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="A10" s="131"/>
+      <c r="A10" s="133"/>
       <c r="B10" s="96" t="s">
         <v>1018</v>
       </c>
@@ -16960,7 +16960,7 @@
       <c r="AH10" s="6"/>
     </row>
     <row r="11" spans="1:34" ht="71" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="132"/>
+      <c r="A11" s="134"/>
       <c r="B11" s="98" t="s">
         <v>1019</v>
       </c>
@@ -17300,7 +17300,7 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="28" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>255</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -17374,7 +17374,7 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="42" x14ac:dyDescent="0.2">
-      <c r="A3" s="134"/>
+      <c r="A3" s="136"/>
       <c r="B3" s="33" t="s">
         <v>323</v>
       </c>
@@ -17446,7 +17446,7 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="70" x14ac:dyDescent="0.2">
-      <c r="A4" s="134"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="33" t="s">
         <v>257</v>
       </c>
@@ -17518,7 +17518,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="135"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="35" t="s">
         <v>326</v>
       </c>

</xml_diff>

<commit_message>
feat: Excel Dateien überarbeitet
</commit_message>
<xml_diff>
--- a/Excel/Übersicht.xlsx
+++ b/Excel/Übersicht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33403420-5907-DA46-B7C0-E41E2D3232BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="10" xr2:uid="{7A4F4436-C796-4ADD-B90F-7338F9426F96}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" firstSheet="1" activeTab="10" xr2:uid="{7A4F4436-C796-4ADD-B90F-7338F9426F96}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="2" state="hidden" r:id="rId1"/>
@@ -8577,19 +8577,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8608,15 +8617,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9383,14 +9383,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="57.36328125" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
@@ -9446,7 +9446,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
@@ -9465,7 +9465,7 @@
       <c r="H5" s="128"/>
       <c r="I5" s="128"/>
     </row>
-    <row r="6" spans="1:9" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21" t="s">
         <v>6</v>
       </c>
@@ -9479,7 +9479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -9499,7 +9499,7 @@
       <c r="H7" s="129"/>
       <c r="I7" s="129"/>
     </row>
-    <row r="8" spans="1:9" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -9517,7 +9517,7 @@
       <c r="H8" s="129"/>
       <c r="I8" s="129"/>
     </row>
-    <row r="9" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -9532,7 +9532,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>Vorwärts aus P2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="66.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="66.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>Rückwärts aus P2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v>Rückwärts aus P2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -9622,7 +9622,7 @@
         <v>Rückwärts aus P2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="19" t="s">
         <v>16</v>
       </c>
@@ -9637,7 +9637,7 @@
         <v>Vorwärts aus P3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17" t="s">
         <v>17</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>Vorwärts aus P4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>Rückwärts aus P4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21" t="s">
         <v>19</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>Vorwärts aus P5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="21" t="s">
         <v>20</v>
       </c>
@@ -9697,7 +9697,7 @@
         <v>Vorwärts aus P5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="21" t="s">
         <v>21</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>Rückwärts aus P5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="36.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="17" t="s">
         <v>22</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>Rückwärts aus P16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="21" t="s">
         <v>23</v>
       </c>
@@ -9742,7 +9742,7 @@
         <v>Rückwärts aus P18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>Vorwärts aus P6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -9772,7 +9772,7 @@
         <v>Vorwärts aus P8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -9787,24 +9787,24 @@
         <v>Vorwärts aus P8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>80</v>
       </c>
@@ -9828,34 +9828,34 @@
       <selection pane="topRight" activeCell="T3" sqref="T3:T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
     <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.453125" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21" customWidth="1"/>
-    <col min="19" max="19" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.83203125" customWidth="1"/>
+    <col min="19" max="19" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="39" t="s">
         <v>238</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" s="135" t="s">
         <v>255</v>
       </c>
@@ -9977,7 +9977,7 @@
       </c>
       <c r="W2" s="27"/>
     </row>
-    <row r="3" spans="1:23" ht="98" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A3" s="136"/>
       <c r="B3" s="33" t="s">
         <v>323</v>
@@ -10034,7 +10034,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="70" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A4" s="136"/>
       <c r="B4" s="33" t="s">
         <v>257</v>
@@ -10085,7 +10085,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="136"/>
       <c r="B5" s="35" t="s">
         <v>326</v>
@@ -10124,7 +10124,7 @@
       <c r="V5" s="29"/>
       <c r="W5" s="30"/>
     </row>
-    <row r="6" spans="1:23" ht="56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="50" x14ac:dyDescent="0.35">
       <c r="A6" s="135" t="s">
         <v>687</v>
       </c>
@@ -10191,7 +10191,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="50" x14ac:dyDescent="0.35">
       <c r="A7" s="136"/>
       <c r="B7" s="33" t="s">
         <v>642</v>
@@ -10240,7 +10240,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="138"/>
       <c r="B8" s="35" t="s">
         <v>592</v>
@@ -10289,7 +10289,7 @@
       <c r="V8" s="29"/>
       <c r="W8" s="30"/>
     </row>
-    <row r="9" spans="1:23" ht="42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A9" s="136" t="s">
         <v>688</v>
       </c>
@@ -10354,7 +10354,7 @@
       </c>
       <c r="W9" s="27"/>
     </row>
-    <row r="10" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="136"/>
       <c r="B10" s="113" t="s">
         <v>962</v>
@@ -10395,7 +10395,7 @@
       </c>
       <c r="W10" s="117"/>
     </row>
-    <row r="11" spans="1:23" ht="42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="50" x14ac:dyDescent="0.35">
       <c r="A11" s="136"/>
       <c r="B11" s="33" t="s">
         <v>963</v>
@@ -10444,7 +10444,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="138"/>
       <c r="B12" s="35" t="s">
         <v>964</v>
@@ -10483,28 +10483,28 @@
       </c>
       <c r="W12" s="30"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="L14" s="78"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="68" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="121" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="18" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="87.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="50.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" ht="50" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" ht="56" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" ht="50" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" ht="50" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" ht="87.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" ht="75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A5"/>
@@ -10521,16 +10521,16 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="4" width="50.1640625" customWidth="1"/>
+    <col min="1" max="2" width="18.36328125" customWidth="1"/>
+    <col min="3" max="4" width="50.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="69" t="s">
         <v>1066</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="125" t="s">
         <v>1070</v>
       </c>
@@ -10558,7 +10558,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="125" t="s">
         <v>1074</v>
       </c>
@@ -10572,7 +10572,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="125" t="s">
         <v>1078</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="125" t="s">
         <v>1082</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="125" t="s">
         <v>1086</v>
       </c>
@@ -10614,7 +10614,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="125" t="s">
         <v>1090</v>
       </c>
@@ -10628,7 +10628,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="74" t="s">
         <v>1094</v>
       </c>
@@ -10642,7 +10642,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="74" t="s">
         <v>1098</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="74" t="s">
         <v>1102</v>
       </c>
@@ -10670,7 +10670,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="74" t="s">
         <v>1106</v>
       </c>
@@ -10684,7 +10684,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="74" t="s">
         <v>1110</v>
       </c>
@@ -10698,7 +10698,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="74" t="s">
         <v>1114</v>
       </c>
@@ -10712,7 +10712,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="74" t="s">
         <v>1118</v>
       </c>
@@ -10739,14 +10739,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.81640625" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>238</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>241</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>243</v>
       </c>
@@ -10777,7 +10777,7 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>245</v>
       </c>
@@ -10786,7 +10786,7 @@
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>246</v>
       </c>
@@ -10809,15 +10809,15 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="138.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="138.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="54" t="s">
         <v>491</v>
       </c>
@@ -10831,32 +10831,32 @@
         <v>494</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="141" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="142" t="s">
         <v>495</v>
       </c>
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="147" t="s">
         <v>496</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="151" t="s">
+      <c r="C2" s="150"/>
+      <c r="D2" s="140" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="143"/>
-      <c r="B3" s="145"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="150"/>
-    </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="142"/>
-      <c r="B4" s="146"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="152"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="141" t="s">
+      <c r="B3" s="148"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="139"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="144"/>
+      <c r="B4" s="149"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="141"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="142" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="58" t="s">
@@ -10869,7 +10869,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="143"/>
       <c r="B6" s="53" t="s">
         <v>499</v>
@@ -10881,7 +10881,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="143"/>
       <c r="B7" s="53" t="s">
         <v>501</v>
@@ -10893,14 +10893,14 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="144"/>
       <c r="B8" s="62"/>
       <c r="C8" s="63"/>
       <c r="D8" s="64"/>
     </row>
-    <row r="9" spans="1:4" ht="28" x14ac:dyDescent="0.2">
-      <c r="A9" s="141" t="s">
+    <row r="9" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+      <c r="A9" s="142" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="58" t="s">
@@ -10913,8 +10913,8 @@
         <v>505</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="142"/>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="144"/>
       <c r="B10" s="82" t="s">
         <v>506</v>
       </c>
@@ -10925,8 +10925,8 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="139" t="s">
+    <row r="11" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="145" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="88" t="s">
@@ -10939,14 +10939,14 @@
         <v>510</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
+    <row r="12" spans="1:4" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="146"/>
       <c r="B12" s="89"/>
       <c r="C12" s="63"/>
       <c r="D12" s="64"/>
     </row>
-    <row r="13" spans="1:4" ht="28" x14ac:dyDescent="0.2">
-      <c r="A13" s="141" t="s">
+    <row r="13" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+      <c r="A13" s="142" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="85" t="s">
@@ -10959,7 +10959,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="143"/>
       <c r="B14" s="53" t="s">
         <v>514</v>
@@ -10971,7 +10971,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="143"/>
       <c r="B15" s="53" t="s">
         <v>474</v>
@@ -10983,26 +10983,26 @@
         <v>518</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="143"/>
-      <c r="B16" s="145"/>
+      <c r="B16" s="148"/>
       <c r="C16" s="52" t="s">
         <v>519</v>
       </c>
-      <c r="D16" s="150" t="s">
+      <c r="D16" s="139" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="143"/>
-      <c r="B17" s="145"/>
+      <c r="B17" s="148"/>
       <c r="C17" s="52" t="s">
         <v>520</v>
       </c>
-      <c r="D17" s="150"/>
-    </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="142"/>
+      <c r="D17" s="139"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="144"/>
       <c r="B18" s="62"/>
       <c r="C18" s="63" t="s">
         <v>522</v>
@@ -11011,8 +11011,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="139" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="145" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="88" t="s">
@@ -11025,14 +11025,14 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="140"/>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="146"/>
       <c r="B20" s="89"/>
       <c r="C20" s="63"/>
       <c r="D20" s="64"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="141" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="142" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="58" t="s">
@@ -11045,26 +11045,26 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="142"/>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="144"/>
       <c r="B22" s="62"/>
       <c r="C22" s="63"/>
       <c r="D22" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11079,34 +11079,34 @@
       <selection pane="topRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" style="14" customWidth="1"/>
     <col min="3" max="3" width="35" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" style="14" customWidth="1"/>
     <col min="5" max="5" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.36328125" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.6640625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.33203125" style="6" customWidth="1"/>
-    <col min="21" max="21" width="38.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.36328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.6328125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="30.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.36328125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="38.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.36328125" style="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="94" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="94" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="37" t="s">
         <v>238</v>
       </c>
@@ -11188,7 +11188,7 @@
       <c r="AG1" s="93"/>
       <c r="AH1" s="93"/>
     </row>
-    <row r="2" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A2" s="135" t="s">
         <v>321</v>
       </c>
@@ -11250,7 +11250,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
     </row>
-    <row r="3" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A3" s="136"/>
       <c r="B3" s="96" t="s">
         <v>252</v>
@@ -11324,7 +11324,7 @@
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
     </row>
-    <row r="4" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A4" s="136"/>
       <c r="B4" s="96" t="s">
         <v>264</v>
@@ -11392,7 +11392,7 @@
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
     </row>
-    <row r="5" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A5" s="136"/>
       <c r="B5" s="96" t="s">
         <v>1015</v>
@@ -11466,7 +11466,7 @@
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
     </row>
-    <row r="6" spans="1:34" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="138"/>
       <c r="B6" s="97" t="s">
         <v>1016</v>
@@ -11534,7 +11534,7 @@
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
     </row>
-    <row r="7" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A7" s="135" t="s">
         <v>320</v>
       </c>
@@ -11612,7 +11612,7 @@
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
     </row>
-    <row r="8" spans="1:34" ht="84" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" ht="75" x14ac:dyDescent="0.35">
       <c r="A8" s="136"/>
       <c r="B8" s="96" t="s">
         <v>997</v>
@@ -11686,7 +11686,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
     </row>
-    <row r="9" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A9" s="136"/>
       <c r="B9" s="96" t="s">
         <v>1017</v>
@@ -11756,7 +11756,7 @@
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
     </row>
-    <row r="10" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A10" s="136"/>
       <c r="B10" s="96" t="s">
         <v>1018</v>
@@ -11826,7 +11826,7 @@
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
     </row>
-    <row r="11" spans="1:34" ht="71" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="63" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="138"/>
       <c r="B11" s="98" t="s">
         <v>1019</v>
@@ -11883,7 +11883,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="135" t="s">
         <v>255</v>
       </c>
@@ -11932,7 +11932,7 @@
       </c>
       <c r="W12" s="27"/>
     </row>
-    <row r="13" spans="1:34" ht="42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A13" s="136"/>
       <c r="B13" s="33" t="s">
         <v>323</v>
@@ -11989,7 +11989,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A14" s="136"/>
       <c r="B14" s="33" t="s">
         <v>257</v>
@@ -12042,7 +12042,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="138"/>
       <c r="B15" s="35" t="s">
         <v>326</v>
@@ -12081,7 +12081,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="30"/>
     </row>
-    <row r="16" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A16" s="135" t="s">
         <v>687</v>
       </c>
@@ -12148,7 +12148,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="56" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" ht="50" x14ac:dyDescent="0.35">
       <c r="A17" s="136"/>
       <c r="B17" s="33" t="s">
         <v>642</v>
@@ -12197,7 +12197,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="138"/>
       <c r="B18" s="35" t="s">
         <v>592</v>
@@ -12246,7 +12246,7 @@
       <c r="V18" s="29"/>
       <c r="W18" s="30"/>
     </row>
-    <row r="19" spans="1:33" ht="42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A19" s="135" t="s">
         <v>688</v>
       </c>
@@ -12311,7 +12311,7 @@
       </c>
       <c r="W19" s="27"/>
     </row>
-    <row r="20" spans="1:33" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="136"/>
       <c r="B20" s="113" t="s">
         <v>962</v>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="W20" s="117"/>
     </row>
-    <row r="21" spans="1:33" ht="42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" ht="50" x14ac:dyDescent="0.35">
       <c r="A21" s="136"/>
       <c r="B21" s="33" t="s">
         <v>963</v>
@@ -12401,7 +12401,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="138"/>
       <c r="B22" s="35" t="s">
         <v>964</v>
@@ -12440,7 +12440,7 @@
       </c>
       <c r="W22" s="30"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
@@ -12464,7 +12464,7 @@
       <c r="AF23" s="14"/>
       <c r="AG23" s="14"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
@@ -12488,7 +12488,7 @@
       <c r="AF24" s="14"/>
       <c r="AG24" s="14"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
@@ -12512,7 +12512,7 @@
       <c r="AF25" s="14"/>
       <c r="AG25" s="14"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
@@ -12536,7 +12536,7 @@
       <c r="AF26" s="14"/>
       <c r="AG26" s="14"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
@@ -12560,7 +12560,7 @@
       <c r="AF27" s="14"/>
       <c r="AG27" s="14"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
@@ -12584,7 +12584,7 @@
       <c r="AF28" s="14"/>
       <c r="AG28" s="14"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
@@ -12608,7 +12608,7 @@
       <c r="AF29" s="14"/>
       <c r="AG29" s="14"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A30" s="14"/>
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
@@ -12654,12 +12654,12 @@
       <selection pane="topRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="23" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C1" s="127" t="s">
         <v>2</v>
       </c>
@@ -12724,7 +12724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="84" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="75" x14ac:dyDescent="0.35">
       <c r="A2" s="135" t="s">
         <v>320</v>
       </c>
@@ -12802,7 +12802,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
     </row>
-    <row r="3" spans="1:34" ht="126" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A3" s="136"/>
       <c r="B3" s="96" t="s">
         <v>997</v>
@@ -12876,7 +12876,7 @@
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
     </row>
-    <row r="4" spans="1:34" ht="98" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A4" s="136"/>
       <c r="B4" s="96" t="s">
         <v>1017</v>
@@ -12946,7 +12946,7 @@
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
     </row>
-    <row r="5" spans="1:34" ht="84" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" ht="75" x14ac:dyDescent="0.35">
       <c r="A5" s="136"/>
       <c r="B5" s="96" t="s">
         <v>1018</v>
@@ -13016,7 +13016,7 @@
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
     </row>
-    <row r="6" spans="1:34" ht="99" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="88" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="138"/>
       <c r="B6" s="98" t="s">
         <v>1019</v>
@@ -13073,7 +13073,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="25" x14ac:dyDescent="0.35">
       <c r="A7" s="135" t="s">
         <v>255</v>
       </c>
@@ -13124,7 +13124,7 @@
       </c>
       <c r="W7" s="27"/>
     </row>
-    <row r="8" spans="1:34" ht="98" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A8" s="136"/>
       <c r="B8" s="33" t="s">
         <v>323</v>
@@ -13181,7 +13181,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="98" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A9" s="136"/>
       <c r="B9" s="33" t="s">
         <v>257</v>
@@ -13232,7 +13232,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="138"/>
       <c r="B10" s="35" t="s">
         <v>326</v>
@@ -13289,22 +13289,22 @@
       <selection activeCell="L1" sqref="L1:R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.6328125" customWidth="1"/>
+    <col min="6" max="6" width="32.36328125" customWidth="1"/>
+    <col min="8" max="8" width="21.36328125" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="17.36328125" customWidth="1"/>
+    <col min="13" max="13" width="26.6328125" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="65" t="s">
         <v>638</v>
       </c>
@@ -13353,7 +13353,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="66" t="s">
         <v>588</v>
       </c>
@@ -13400,7 +13400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="66" t="s">
         <v>589</v>
       </c>
@@ -13447,7 +13447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="66" t="s">
         <v>591</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="66" t="s">
         <v>593</v>
       </c>
@@ -13532,7 +13532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="66" t="s">
         <v>595</v>
       </c>
@@ -13579,7 +13579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="66" t="s">
         <v>597</v>
       </c>
@@ -13617,7 +13617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="66" t="s">
         <v>599</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="66" t="s">
         <v>601</v>
       </c>
@@ -13663,7 +13663,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="66" t="s">
         <v>603</v>
       </c>
@@ -13677,7 +13677,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="66" t="s">
         <v>605</v>
       </c>
@@ -13700,7 +13700,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="49" t="s">
         <v>607</v>
       </c>
@@ -13723,7 +13723,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D13" s="66" t="s">
         <v>602</v>
       </c>
@@ -13740,7 +13740,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D14" s="66" t="s">
         <v>598</v>
       </c>
@@ -13751,7 +13751,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="D15" s="49" t="s">
         <v>625</v>
       </c>
@@ -13762,7 +13762,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D16" s="66" t="s">
         <v>627</v>
       </c>
@@ -13782,18 +13782,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBF0DFC-ABCB-4798-A2A7-A9FED467CFB2}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
     <col min="3" max="3" width="74" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
         <v>74</v>
       </c>
@@ -13807,7 +13807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>2</v>
       </c>
@@ -13827,7 +13827,7 @@
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="46" t="s">
         <v>3</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="46" t="s">
         <v>4</v>
       </c>
@@ -13858,7 +13858,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="46" t="s">
         <v>5</v>
       </c>
@@ -13872,7 +13872,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
@@ -13887,7 +13887,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
@@ -13902,7 +13902,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
@@ -13917,7 +13917,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -13947,7 +13947,7 @@
         <v>Rückwärts aus P1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="19" t="s">
         <v>11</v>
       </c>
@@ -13961,7 +13961,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>Vorwärts aus P2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -13991,7 +13991,7 @@
         <v>Rückwärts aus P2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="19" t="s">
         <v>14</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>Rückwärts aus P2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="19" t="s">
         <v>15</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>Rückwärts aus P3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="19" t="s">
         <v>16</v>
       </c>
@@ -14036,7 +14036,7 @@
         <v>Rückwärts aus P3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="19" t="s">
         <v>17</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="23" t="s">
         <v>18</v>
       </c>
@@ -14065,7 +14065,7 @@
         <v>Vorwärts aus P5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
@@ -14079,7 +14079,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="23" t="s">
         <v>20</v>
       </c>
@@ -14093,7 +14093,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="23" t="s">
         <v>21</v>
       </c>
@@ -14108,7 +14108,7 @@
         <v>Vorwärts aus P7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="23" t="s">
         <v>22</v>
       </c>
@@ -14122,14 +14122,14 @@
         <v>283</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
     </row>
   </sheetData>
@@ -14146,20 +14146,20 @@
       <selection activeCell="A12" sqref="A12:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="50.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="35.83203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="14.1796875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="29.6328125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="32.6328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="50.81640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="35.81640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="10.81640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -14185,7 +14185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -14211,7 +14211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -14237,7 +14237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="71" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -14263,7 +14263,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -14289,7 +14289,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -14315,7 +14315,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -14341,7 +14341,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -14367,7 +14367,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -14393,7 +14393,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -14419,7 +14419,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -14445,7 +14445,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -14471,7 +14471,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -14497,7 +14497,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -14523,7 +14523,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -14549,7 +14549,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -14575,7 +14575,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -14601,7 +14601,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -14627,7 +14627,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -14653,7 +14653,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -14679,7 +14679,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -14705,7 +14705,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -14731,7 +14731,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
@@ -14757,7 +14757,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -14783,7 +14783,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -14809,7 +14809,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -14835,7 +14835,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
@@ -14850,14 +14850,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H28" s="6">
         <f>Übersicht!D28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
@@ -14865,7 +14865,7 @@
       <c r="E39" s="10"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
@@ -14889,18 +14889,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6328125" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>261</v>
       </c>
@@ -14921,7 +14921,7 @@
       <c r="J1" s="130"/>
       <c r="K1" s="130"/>
     </row>
-    <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>251</v>
       </c>
@@ -14942,7 +14942,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>252</v>
       </c>
@@ -14961,7 +14961,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>264</v>
       </c>
@@ -14980,7 +14980,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>253</v>
       </c>
@@ -14999,7 +14999,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>254</v>
       </c>
@@ -15018,7 +15018,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>265</v>
       </c>
@@ -15037,14 +15037,14 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -15068,15 +15068,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" customWidth="1"/>
-    <col min="4" max="4" width="61.5" customWidth="1"/>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" customWidth="1"/>
+    <col min="3" max="3" width="54.36328125" customWidth="1"/>
+    <col min="4" max="4" width="61.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>261</v>
       </c>
@@ -15090,7 +15090,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="50" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>251</v>
       </c>
@@ -15104,7 +15104,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="50" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>252</v>
       </c>
@@ -15118,7 +15118,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>264</v>
       </c>
@@ -15132,7 +15132,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>253</v>
       </c>
@@ -15146,7 +15146,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>254</v>
       </c>
@@ -15160,7 +15160,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>265</v>
       </c>
@@ -15187,14 +15187,14 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" style="12" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="4" width="53.5" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
+    <col min="3" max="4" width="53.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
@@ -15210,7 +15210,7 @@
       <c r="E1" s="103"/>
       <c r="F1" s="103"/>
     </row>
-    <row r="2" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A2" s="104" t="s">
         <v>2</v>
       </c>
@@ -15226,7 +15226,7 @@
       <c r="E2" s="78"/>
       <c r="F2" s="78"/>
     </row>
-    <row r="3" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A3" s="104" t="s">
         <v>3</v>
       </c>
@@ -15242,7 +15242,7 @@
       <c r="E3" s="78"/>
       <c r="F3" s="78"/>
     </row>
-    <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A4" s="104" t="s">
         <v>4</v>
       </c>
@@ -15258,7 +15258,7 @@
       <c r="E4" s="78"/>
       <c r="F4" s="78"/>
     </row>
-    <row r="5" spans="1:6" ht="84" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.35">
       <c r="A5" s="104" t="s">
         <v>5</v>
       </c>
@@ -15274,7 +15274,7 @@
       <c r="E5" s="78"/>
       <c r="F5" s="78"/>
     </row>
-    <row r="6" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A6" s="104" t="s">
         <v>6</v>
       </c>
@@ -15290,7 +15290,7 @@
       <c r="E6" s="78"/>
       <c r="F6" s="78"/>
     </row>
-    <row r="7" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A7" s="104" t="s">
         <v>7</v>
       </c>
@@ -15306,7 +15306,7 @@
       <c r="E7" s="78"/>
       <c r="F7" s="78"/>
     </row>
-    <row r="8" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A8" s="104" t="s">
         <v>8</v>
       </c>
@@ -15322,7 +15322,7 @@
       <c r="E8" s="78"/>
       <c r="F8" s="78"/>
     </row>
-    <row r="9" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A9" s="104" t="s">
         <v>9</v>
       </c>
@@ -15338,7 +15338,7 @@
       <c r="E9" s="78"/>
       <c r="F9" s="78"/>
     </row>
-    <row r="10" spans="1:6" ht="42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="104" t="s">
         <v>10</v>
       </c>
@@ -15354,7 +15354,7 @@
       <c r="E10" s="78"/>
       <c r="F10" s="78"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="104" t="s">
         <v>10</v>
       </c>
@@ -15364,7 +15364,7 @@
       <c r="E11" s="78"/>
       <c r="F11" s="78"/>
     </row>
-    <row r="12" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A12" s="104" t="s">
         <v>11</v>
       </c>
@@ -15380,7 +15380,7 @@
       <c r="E12" s="78"/>
       <c r="F12" s="78"/>
     </row>
-    <row r="13" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A13" s="104" t="s">
         <v>12</v>
       </c>
@@ -15396,7 +15396,7 @@
       <c r="E13" s="78"/>
       <c r="F13" s="78"/>
     </row>
-    <row r="14" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A14" s="104" t="s">
         <v>13</v>
       </c>
@@ -15412,7 +15412,7 @@
       <c r="E14" s="78"/>
       <c r="F14" s="78"/>
     </row>
-    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="25" x14ac:dyDescent="0.35">
       <c r="A15" s="104" t="s">
         <v>14</v>
       </c>
@@ -15428,7 +15428,7 @@
       <c r="E15" s="78"/>
       <c r="F15" s="78"/>
     </row>
-    <row r="16" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="100" x14ac:dyDescent="0.35">
       <c r="A16" s="104" t="s">
         <v>15</v>
       </c>
@@ -15444,7 +15444,7 @@
       <c r="E16" s="78"/>
       <c r="F16" s="78"/>
     </row>
-    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A17" s="104" t="s">
         <v>16</v>
       </c>
@@ -15460,7 +15460,7 @@
       <c r="E17" s="78"/>
       <c r="F17" s="78"/>
     </row>
-    <row r="18" spans="1:6" ht="70" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="104" t="s">
         <v>18</v>
       </c>
@@ -15476,7 +15476,7 @@
       <c r="E18" s="78"/>
       <c r="F18" s="78"/>
     </row>
-    <row r="19" spans="1:6" ht="42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A19" s="104" t="s">
         <v>17</v>
       </c>
@@ -15492,7 +15492,7 @@
       <c r="E19" s="78"/>
       <c r="F19" s="78"/>
     </row>
-    <row r="20" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A20" s="104" t="s">
         <v>18</v>
       </c>
@@ -15508,7 +15508,7 @@
       <c r="E20" s="78"/>
       <c r="F20" s="78"/>
     </row>
-    <row r="21" spans="1:6" ht="42" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="104" t="s">
         <v>21</v>
       </c>
@@ -15524,7 +15524,7 @@
       <c r="E21" s="78"/>
       <c r="F21" s="78"/>
     </row>
-    <row r="22" spans="1:6" ht="56" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="50" x14ac:dyDescent="0.35">
       <c r="A22" s="104" t="s">
         <v>19</v>
       </c>
@@ -15540,7 +15540,7 @@
       <c r="E22" s="78"/>
       <c r="F22" s="78"/>
     </row>
-    <row r="23" spans="1:6" ht="70" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A23" s="104" t="s">
         <v>20</v>
       </c>
@@ -15556,15 +15556,15 @@
       <c r="E23" s="78"/>
       <c r="F23" s="78"/>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="E25" s="78"/>
       <c r="F25" s="78"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="109" t="s">
         <v>21</v>
       </c>
@@ -15574,7 +15574,7 @@
       <c r="E26" s="78"/>
       <c r="F26" s="78"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="109" t="s">
         <v>3</v>
       </c>
@@ -15599,30 +15599,30 @@
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
     <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.83203125" customWidth="1"/>
-    <col min="10" max="10" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.81640625" customWidth="1"/>
+    <col min="10" max="10" width="38.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="36.83203125" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="36.83203125" customWidth="1"/>
-    <col min="22" max="22" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="36.81640625" customWidth="1"/>
+    <col min="19" max="19" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="36.81640625" customWidth="1"/>
+    <col min="22" max="22" width="37.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="50" t="s">
         <v>238</v>
       </c>
@@ -15690,7 +15690,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="70" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
         <v>470</v>
       </c>
@@ -15758,7 +15758,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="154" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="139" x14ac:dyDescent="0.35">
       <c r="A3" s="50" t="s">
         <v>81</v>
       </c>
@@ -15826,7 +15826,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="140" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A4" s="50" t="s">
         <v>471</v>
       </c>
@@ -15894,7 +15894,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="50" t="s">
         <v>472</v>
       </c>
@@ -15962,7 +15962,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="154" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="139" x14ac:dyDescent="0.35">
       <c r="A6" s="50" t="s">
         <v>475</v>
       </c>
@@ -16030,7 +16030,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="70" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A7" s="50" t="s">
         <v>473</v>
       </c>
@@ -16098,7 +16098,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="100" x14ac:dyDescent="0.35">
       <c r="A8" s="50" t="s">
         <v>474</v>
       </c>
@@ -16166,31 +16166,31 @@
         <v>578</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B13" s="131"/>
       <c r="C13" s="131"/>
       <c r="G13" s="67"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B14" s="131"/>
       <c r="C14" s="131"/>
       <c r="G14" s="67"/>
     </row>
-    <row r="15" spans="1:22" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="100.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="131"/>
       <c r="C15" s="131"/>
       <c r="G15" s="67"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G16" s="67"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17" s="67"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G18" s="67"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19" s="67"/>
     </row>
   </sheetData>
@@ -16212,34 +16212,34 @@
       <selection pane="topRight" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" style="14" customWidth="1"/>
     <col min="3" max="3" width="35" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" style="14" customWidth="1"/>
     <col min="5" max="5" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.36328125" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.6640625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.33203125" style="6" customWidth="1"/>
-    <col min="21" max="21" width="38.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.36328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.6328125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="30.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.36328125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="38.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.36328125" style="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="94" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="94" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="37" t="s">
         <v>238</v>
       </c>
@@ -16321,7 +16321,7 @@
       <c r="AG1" s="93"/>
       <c r="AH1" s="93"/>
     </row>
-    <row r="2" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A2" s="135" t="s">
         <v>321</v>
       </c>
@@ -16383,7 +16383,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
     </row>
-    <row r="3" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A3" s="136"/>
       <c r="B3" s="96" t="s">
         <v>252</v>
@@ -16457,7 +16457,7 @@
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
     </row>
-    <row r="4" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A4" s="136"/>
       <c r="B4" s="96" t="s">
         <v>264</v>
@@ -16525,7 +16525,7 @@
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
     </row>
-    <row r="5" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A5" s="136"/>
       <c r="B5" s="96" t="s">
         <v>1015</v>
@@ -16599,7 +16599,7 @@
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
     </row>
-    <row r="6" spans="1:34" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="136"/>
       <c r="B6" s="97" t="s">
         <v>1016</v>
@@ -16667,7 +16667,7 @@
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
     </row>
-    <row r="7" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A7" s="132" t="s">
         <v>320</v>
       </c>
@@ -16745,7 +16745,7 @@
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
     </row>
-    <row r="8" spans="1:34" ht="84" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" ht="75" x14ac:dyDescent="0.35">
       <c r="A8" s="133"/>
       <c r="B8" s="96" t="s">
         <v>997</v>
@@ -16819,7 +16819,7 @@
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
     </row>
-    <row r="9" spans="1:34" ht="70" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A9" s="133"/>
       <c r="B9" s="96" t="s">
         <v>1017</v>
@@ -16889,7 +16889,7 @@
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
     </row>
-    <row r="10" spans="1:34" ht="56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" ht="50" x14ac:dyDescent="0.35">
       <c r="A10" s="133"/>
       <c r="B10" s="96" t="s">
         <v>1018</v>
@@ -16959,7 +16959,7 @@
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
     </row>
-    <row r="11" spans="1:34" ht="71" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="63" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="134"/>
       <c r="B11" s="98" t="s">
         <v>1019</v>
@@ -17016,7 +17016,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -17025,12 +17025,12 @@
       <c r="U15"/>
       <c r="V15"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="L16" s="6"/>
       <c r="U16"/>
       <c r="V16"/>
     </row>
-    <row r="17" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="9:22" x14ac:dyDescent="0.35">
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -17041,7 +17041,7 @@
       <c r="U17"/>
       <c r="V17"/>
     </row>
-    <row r="18" spans="9:22" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="9:22" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -17055,7 +17055,7 @@
       <c r="U18"/>
       <c r="V18"/>
     </row>
-    <row r="19" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -17069,7 +17069,7 @@
       <c r="U19"/>
       <c r="V19"/>
     </row>
-    <row r="20" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -17083,7 +17083,7 @@
       <c r="U20"/>
       <c r="V20"/>
     </row>
-    <row r="21" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -17097,7 +17097,7 @@
       <c r="U21"/>
       <c r="V21"/>
     </row>
-    <row r="22" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -17111,7 +17111,7 @@
       <c r="U22"/>
       <c r="V22"/>
     </row>
-    <row r="23" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -17125,7 +17125,7 @@
       <c r="U23"/>
       <c r="V23"/>
     </row>
-    <row r="24" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
@@ -17139,7 +17139,7 @@
       <c r="U24"/>
       <c r="V24"/>
     </row>
-    <row r="25" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="9:22" x14ac:dyDescent="0.35">
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -17153,7 +17153,7 @@
       <c r="U25"/>
       <c r="V25"/>
     </row>
-    <row r="26" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="9:22" x14ac:dyDescent="0.35">
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="Q26" s="14"/>
@@ -17163,7 +17163,7 @@
       <c r="U26"/>
       <c r="V26"/>
     </row>
-    <row r="27" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="9:22" x14ac:dyDescent="0.35">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="Q27" s="14"/>
@@ -17173,7 +17173,7 @@
       <c r="U27"/>
       <c r="V27"/>
     </row>
-    <row r="28" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="9:22" x14ac:dyDescent="0.35">
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
       <c r="U28" s="14"/>
@@ -17198,34 +17198,34 @@
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.33203125" customWidth="1"/>
-    <col min="11" max="11" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="47.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.83203125" customWidth="1"/>
-    <col min="18" max="18" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.36328125" customWidth="1"/>
+    <col min="11" max="11" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.81640625" customWidth="1"/>
+    <col min="18" max="18" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" customWidth="1"/>
-    <col min="20" max="20" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="25.1640625" customWidth="1"/>
-    <col min="23" max="23" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.83203125" customWidth="1"/>
+    <col min="20" max="20" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="25.1796875" customWidth="1"/>
+    <col min="23" max="23" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="39" t="s">
         <v>238</v>
       </c>
@@ -17299,7 +17299,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" s="135" t="s">
         <v>255</v>
       </c>
@@ -17373,7 +17373,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A3" s="136"/>
       <c r="B3" s="33" t="s">
         <v>323</v>
@@ -17445,7 +17445,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="70" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A4" s="136"/>
       <c r="B4" s="33" t="s">
         <v>257</v>
@@ -17517,7 +17517,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="137"/>
       <c r="B5" s="35" t="s">
         <v>326</v>
@@ -17589,7 +17589,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A6" s="75" t="s">
         <v>357</v>
       </c>
@@ -17663,7 +17663,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A7" s="76"/>
       <c r="B7" s="33" t="s">
         <v>332</v>
@@ -17735,7 +17735,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A8" s="76"/>
       <c r="B8" s="33" t="s">
         <v>333</v>
@@ -17807,7 +17807,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A9" s="76"/>
       <c r="B9" s="33" t="s">
         <v>259</v>
@@ -17879,7 +17879,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="50" x14ac:dyDescent="0.35">
       <c r="A10" s="76"/>
       <c r="B10" s="33" t="s">
         <v>337</v>
@@ -17951,7 +17951,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="84" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="75" x14ac:dyDescent="0.35">
       <c r="A11" s="76"/>
       <c r="B11" s="33" t="s">
         <v>339</v>
@@ -18023,7 +18023,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="77"/>
       <c r="B12" s="35" t="s">
         <v>260</v>
@@ -18095,15 +18095,15 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="56" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="87.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="50.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" ht="50" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" ht="56" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" ht="34" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" ht="50" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" ht="50" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" ht="87.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" ht="75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" ht="50.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A5"/>

</xml_diff>